<commit_message>
extracting + cleaning audit data
</commit_message>
<xml_diff>
--- a/data/audit/bs/bs_core.xlsx
+++ b/data/audit/bs/bs_core.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Fix: extracting units in requirements
</commit_message>
<xml_diff>
--- a/data/audit/bs/bs_core.xlsx
+++ b/data/audit/bs/bs_core.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B219"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>course</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>min_units</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,6 +461,9 @@
           <t>03-121</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +476,9 @@
           <t>03-151</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -480,6 +491,9 @@
           <t>03-201</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -492,6 +506,9 @@
           <t>03-202</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -504,6 +521,9 @@
           <t>03-301</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -516,6 +536,9 @@
           <t>03-302</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -528,6 +551,9 @@
           <t>03-401</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -540,6 +566,9 @@
           <t>03-402</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -552,6 +581,9 @@
           <t>03-220</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -564,6 +596,9 @@
           <t>03-231</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -576,6 +611,9 @@
           <t>03-232</t>
         </is>
       </c>
+      <c r="C12" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -588,6 +626,9 @@
           <t>02-250</t>
         </is>
       </c>
+      <c r="C13" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -600,6 +641,9 @@
           <t>03-250</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -612,6 +656,9 @@
           <t>03-251</t>
         </is>
       </c>
+      <c r="C15" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -624,6 +671,9 @@
           <t>03-252</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -636,6 +686,9 @@
           <t>03-240</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -648,6 +701,9 @@
           <t>03-320</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -660,6 +716,9 @@
           <t>03-343</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -672,6 +731,9 @@
           <t>03-344</t>
         </is>
       </c>
+      <c r="C20" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -684,6 +746,9 @@
           <t>03-345</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -696,6 +761,9 @@
           <t>03-346</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -708,6 +776,9 @@
           <t>03-411</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -720,6 +791,9 @@
           <t>03-412</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -732,6 +806,9 @@
           <t>03-326</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -744,6 +821,9 @@
           <t>03-327</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -756,6 +836,9 @@
           <t>03-350</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -768,6 +851,9 @@
           <t>03-362</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -780,6 +866,9 @@
           <t>03-363</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -792,6 +881,9 @@
           <t>03-364</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -804,6 +896,9 @@
           <t>03-365</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -816,6 +911,9 @@
           <t>03-366</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -828,6 +926,9 @@
           <t>03-380</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -840,6 +941,9 @@
           <t>03-390</t>
         </is>
       </c>
+      <c r="C34" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -852,6 +956,9 @@
           <t>03-391</t>
         </is>
       </c>
+      <c r="C35" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -864,6 +971,9 @@
           <t>03-392</t>
         </is>
       </c>
+      <c r="C36" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -876,6 +986,9 @@
           <t>03-410</t>
         </is>
       </c>
+      <c r="C37" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -888,6 +1001,9 @@
           <t>03-428</t>
         </is>
       </c>
+      <c r="C38" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -900,6 +1016,9 @@
           <t>03-435</t>
         </is>
       </c>
+      <c r="C39" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -912,6 +1031,9 @@
           <t>03-439</t>
         </is>
       </c>
+      <c r="C40" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -924,6 +1046,9 @@
           <t>03-442</t>
         </is>
       </c>
+      <c r="C41" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -936,6 +1061,9 @@
           <t>03-451</t>
         </is>
       </c>
+      <c r="C42" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -948,6 +1076,9 @@
           <t>03-511</t>
         </is>
       </c>
+      <c r="C43" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -960,6 +1091,9 @@
           <t>03-512</t>
         </is>
       </c>
+      <c r="C44" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -972,6 +1106,9 @@
           <t>03-534</t>
         </is>
       </c>
+      <c r="C45" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -984,6 +1121,9 @@
           <t>03-620</t>
         </is>
       </c>
+      <c r="C46" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -996,6 +1136,9 @@
           <t>03-709</t>
         </is>
       </c>
+      <c r="C47" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1008,6 +1151,9 @@
           <t>03-711</t>
         </is>
       </c>
+      <c r="C48" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1020,6 +1166,9 @@
           <t>03-712</t>
         </is>
       </c>
+      <c r="C49" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1032,6 +1181,9 @@
           <t>03-713</t>
         </is>
       </c>
+      <c r="C50" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1044,6 +1196,9 @@
           <t>03-726</t>
         </is>
       </c>
+      <c r="C51" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1056,6 +1211,9 @@
           <t>03-727</t>
         </is>
       </c>
+      <c r="C52" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1068,6 +1226,9 @@
           <t>03-728</t>
         </is>
       </c>
+      <c r="C53" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1080,6 +1241,9 @@
           <t>03-730</t>
         </is>
       </c>
+      <c r="C54" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1092,6 +1256,9 @@
           <t>03-740</t>
         </is>
       </c>
+      <c r="C55" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1104,6 +1271,9 @@
           <t>03-741</t>
         </is>
       </c>
+      <c r="C56" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1116,6 +1286,9 @@
           <t>03-742</t>
         </is>
       </c>
+      <c r="C57" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1128,6 +1301,9 @@
           <t>03-744</t>
         </is>
       </c>
+      <c r="C58" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1140,6 +1316,9 @@
           <t>03-751</t>
         </is>
       </c>
+      <c r="C59" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1152,6 +1331,9 @@
           <t>03-760</t>
         </is>
       </c>
+      <c r="C60" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1164,6 +1346,9 @@
           <t>03-762</t>
         </is>
       </c>
+      <c r="C61" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1176,6 +1361,9 @@
           <t>03-763</t>
         </is>
       </c>
+      <c r="C62" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1188,6 +1376,9 @@
           <t>03-765</t>
         </is>
       </c>
+      <c r="C63" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1200,6 +1391,9 @@
           <t>03-770</t>
         </is>
       </c>
+      <c r="C64" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1212,6 +1406,9 @@
           <t>03-791</t>
         </is>
       </c>
+      <c r="C65" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1224,6 +1421,9 @@
           <t>03-871</t>
         </is>
       </c>
+      <c r="C66" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1236,6 +1436,9 @@
           <t>03-115</t>
         </is>
       </c>
+      <c r="C67" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1248,6 +1451,9 @@
           <t>03-116</t>
         </is>
       </c>
+      <c r="C68" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1260,6 +1466,9 @@
           <t>03-124</t>
         </is>
       </c>
+      <c r="C69" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1272,6 +1481,9 @@
           <t>03-125</t>
         </is>
       </c>
+      <c r="C70" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1284,6 +1496,9 @@
           <t>03-126</t>
         </is>
       </c>
+      <c r="C71" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1296,6 +1511,9 @@
           <t>03-127</t>
         </is>
       </c>
+      <c r="C72" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1308,6 +1526,9 @@
           <t>03-133</t>
         </is>
       </c>
+      <c r="C73" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1320,6 +1541,9 @@
           <t>03-161</t>
         </is>
       </c>
+      <c r="C74" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1332,6 +1556,9 @@
           <t>03-326</t>
         </is>
       </c>
+      <c r="C75" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1344,6 +1571,9 @@
           <t>03-327</t>
         </is>
       </c>
+      <c r="C76" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1356,6 +1586,9 @@
           <t>03-350</t>
         </is>
       </c>
+      <c r="C77" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1368,6 +1601,9 @@
           <t>03-362</t>
         </is>
       </c>
+      <c r="C78" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1380,6 +1616,9 @@
           <t>03-363</t>
         </is>
       </c>
+      <c r="C79" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1392,6 +1631,9 @@
           <t>03-364</t>
         </is>
       </c>
+      <c r="C80" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1404,6 +1646,9 @@
           <t>03-365</t>
         </is>
       </c>
+      <c r="C81" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1416,6 +1661,9 @@
           <t>03-366</t>
         </is>
       </c>
+      <c r="C82" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1428,6 +1676,9 @@
           <t>03-370</t>
         </is>
       </c>
+      <c r="C83" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1440,6 +1691,9 @@
           <t>03-390</t>
         </is>
       </c>
+      <c r="C84" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1452,6 +1706,9 @@
           <t>03-391</t>
         </is>
       </c>
+      <c r="C85" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1464,6 +1721,9 @@
           <t>03-392</t>
         </is>
       </c>
+      <c r="C86" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1476,6 +1736,9 @@
           <t>03-428</t>
         </is>
       </c>
+      <c r="C87" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1488,6 +1751,9 @@
           <t>03-435</t>
         </is>
       </c>
+      <c r="C88" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1500,6 +1766,9 @@
           <t>03-439</t>
         </is>
       </c>
+      <c r="C89" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1512,6 +1781,9 @@
           <t>03-442</t>
         </is>
       </c>
+      <c r="C90" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1524,6 +1796,9 @@
           <t>03-451</t>
         </is>
       </c>
+      <c r="C91" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1536,6 +1811,9 @@
           <t>03-511</t>
         </is>
       </c>
+      <c r="C92" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1548,6 +1826,9 @@
           <t>03-512</t>
         </is>
       </c>
+      <c r="C93" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1560,6 +1841,9 @@
           <t>03-534</t>
         </is>
       </c>
+      <c r="C94" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1572,6 +1856,9 @@
           <t>03-620</t>
         </is>
       </c>
+      <c r="C95" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1584,6 +1871,9 @@
           <t>03-709</t>
         </is>
       </c>
+      <c r="C96" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1596,6 +1886,9 @@
           <t>03-711</t>
         </is>
       </c>
+      <c r="C97" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1608,6 +1901,9 @@
           <t>03-712</t>
         </is>
       </c>
+      <c r="C98" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1620,6 +1916,9 @@
           <t>03-713</t>
         </is>
       </c>
+      <c r="C99" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1632,6 +1931,9 @@
           <t>03-726</t>
         </is>
       </c>
+      <c r="C100" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1644,6 +1946,9 @@
           <t>03-727</t>
         </is>
       </c>
+      <c r="C101" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1656,6 +1961,9 @@
           <t>03-728</t>
         </is>
       </c>
+      <c r="C102" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1668,6 +1976,9 @@
           <t>03-730</t>
         </is>
       </c>
+      <c r="C103" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1680,6 +1991,9 @@
           <t>03-740</t>
         </is>
       </c>
+      <c r="C104" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1692,6 +2006,9 @@
           <t>03-741</t>
         </is>
       </c>
+      <c r="C105" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1704,6 +2021,9 @@
           <t>03-742</t>
         </is>
       </c>
+      <c r="C106" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1716,6 +2036,9 @@
           <t>03-744</t>
         </is>
       </c>
+      <c r="C107" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1728,6 +2051,9 @@
           <t>03-751</t>
         </is>
       </c>
+      <c r="C108" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1740,6 +2066,9 @@
           <t>03-762</t>
         </is>
       </c>
+      <c r="C109" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1752,6 +2081,9 @@
           <t>03-763</t>
         </is>
       </c>
+      <c r="C110" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1764,6 +2096,9 @@
           <t>03-765</t>
         </is>
       </c>
+      <c r="C111" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1776,6 +2111,9 @@
           <t>03-770</t>
         </is>
       </c>
+      <c r="C112" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1788,6 +2126,9 @@
           <t>03-791</t>
         </is>
       </c>
+      <c r="C113" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1800,6 +2141,9 @@
           <t>03-871</t>
         </is>
       </c>
+      <c r="C114" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1812,6 +2156,9 @@
           <t>03-113</t>
         </is>
       </c>
+      <c r="C115" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -1824,6 +2171,9 @@
           <t>03-117</t>
         </is>
       </c>
+      <c r="C116" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -1836,6 +2186,9 @@
           <t>03-230</t>
         </is>
       </c>
+      <c r="C117" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -1848,6 +2201,9 @@
           <t>03-120</t>
         </is>
       </c>
+      <c r="C118" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1860,6 +2216,9 @@
           <t>03-118</t>
         </is>
       </c>
+      <c r="C119" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -1872,6 +2231,9 @@
           <t>03-445</t>
         </is>
       </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -1884,6 +2246,9 @@
           <t>03-545</t>
         </is>
       </c>
+      <c r="C121" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -1896,6 +2261,9 @@
           <t>09-518</t>
         </is>
       </c>
+      <c r="C122" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -1908,6 +2276,9 @@
           <t>09-519</t>
         </is>
       </c>
+      <c r="C123" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -1920,6 +2291,9 @@
           <t>09-521</t>
         </is>
       </c>
+      <c r="C124" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -1932,6 +2306,9 @@
           <t>21-127</t>
         </is>
       </c>
+      <c r="C125" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -1944,6 +2321,9 @@
           <t>21-128</t>
         </is>
       </c>
+      <c r="C126" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -1956,6 +2336,9 @@
           <t>21-259</t>
         </is>
       </c>
+      <c r="C127" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -1968,6 +2351,9 @@
           <t>36-200</t>
         </is>
       </c>
+      <c r="C128" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -1980,6 +2366,9 @@
           <t>21-260</t>
         </is>
       </c>
+      <c r="C129" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -1992,6 +2381,9 @@
           <t>36-201</t>
         </is>
       </c>
+      <c r="C130" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2004,6 +2396,9 @@
           <t>36-247</t>
         </is>
       </c>
+      <c r="C131" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2016,6 +2411,9 @@
           <t>42-202</t>
         </is>
       </c>
+      <c r="C132" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2028,6 +2426,9 @@
           <t>85-219</t>
         </is>
       </c>
+      <c r="C133" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2040,6 +2441,9 @@
           <t>09-105</t>
         </is>
       </c>
+      <c r="C134" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2052,6 +2456,9 @@
           <t>09-107</t>
         </is>
       </c>
+      <c r="C135" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2064,6 +2471,9 @@
           <t>09-106</t>
         </is>
       </c>
+      <c r="C136" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2076,6 +2486,9 @@
           <t>09-217</t>
         </is>
       </c>
+      <c r="C137" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2088,6 +2501,9 @@
           <t>09-219</t>
         </is>
       </c>
+      <c r="C138" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2100,6 +2516,9 @@
           <t>09-218</t>
         </is>
       </c>
+      <c r="C139" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2112,6 +2531,9 @@
           <t>09-220</t>
         </is>
       </c>
+      <c r="C140" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2124,6 +2546,9 @@
           <t>09-207</t>
         </is>
       </c>
+      <c r="C141" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2136,6 +2561,9 @@
           <t>09-221</t>
         </is>
       </c>
+      <c r="C142" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2148,6 +2576,9 @@
           <t>09-208</t>
         </is>
       </c>
+      <c r="C143" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2160,6 +2591,9 @@
           <t>09-222</t>
         </is>
       </c>
+      <c r="C144" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2172,6 +2606,9 @@
           <t>QC-211</t>
         </is>
       </c>
+      <c r="C145" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2184,6 +2621,9 @@
           <t>02-201</t>
         </is>
       </c>
+      <c r="C146" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2196,6 +2636,9 @@
           <t>15-110</t>
         </is>
       </c>
+      <c r="C147" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2208,6 +2651,9 @@
           <t>15-112</t>
         </is>
       </c>
+      <c r="C148" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2220,6 +2666,9 @@
           <t>21-112</t>
         </is>
       </c>
+      <c r="C149" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2232,6 +2681,9 @@
           <t>21-120</t>
         </is>
       </c>
+      <c r="C150" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2244,6 +2696,9 @@
           <t>21-122</t>
         </is>
       </c>
+      <c r="C151" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2256,6 +2711,9 @@
           <t>21-124</t>
         </is>
       </c>
+      <c r="C152" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2268,6 +2726,9 @@
           <t>33-111</t>
         </is>
       </c>
+      <c r="C153" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -2280,6 +2741,9 @@
           <t>33-121</t>
         </is>
       </c>
+      <c r="C154" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2292,6 +2756,9 @@
           <t>33-141</t>
         </is>
       </c>
+      <c r="C155" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2304,6 +2771,9 @@
           <t>33-151</t>
         </is>
       </c>
+      <c r="C156" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2316,6 +2786,9 @@
           <t>33-112</t>
         </is>
       </c>
+      <c r="C157" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2328,6 +2801,9 @@
           <t>33-122</t>
         </is>
       </c>
+      <c r="C158" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2340,6 +2816,9 @@
           <t>33-142</t>
         </is>
       </c>
+      <c r="C159" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2352,6 +2831,9 @@
           <t>33-152</t>
         </is>
       </c>
+      <c r="C160" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2364,6 +2846,9 @@
           <t>99-101</t>
         </is>
       </c>
+      <c r="C161" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2376,6 +2861,9 @@
           <t>99-102</t>
         </is>
       </c>
+      <c r="C162" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2388,6 +2876,9 @@
           <t>03-740</t>
         </is>
       </c>
+      <c r="C163" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2400,6 +2891,9 @@
           <t>21-259</t>
         </is>
       </c>
+      <c r="C164" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2412,6 +2906,9 @@
           <t>21-260</t>
         </is>
       </c>
+      <c r="C165" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2424,6 +2921,9 @@
           <t>09-518</t>
         </is>
       </c>
+      <c r="C166" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -2436,6 +2936,9 @@
           <t>09-519</t>
         </is>
       </c>
+      <c r="C167" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -2448,6 +2951,9 @@
           <t>09-521</t>
         </is>
       </c>
+      <c r="C168" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -2460,6 +2966,9 @@
           <t>03-442</t>
         </is>
       </c>
+      <c r="C169" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -2472,6 +2981,9 @@
           <t>03-534</t>
         </is>
       </c>
+      <c r="C170" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -2484,6 +2996,9 @@
           <t>03-439</t>
         </is>
       </c>
+      <c r="C171" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -2496,6 +3011,9 @@
           <t>03-871</t>
         </is>
       </c>
+      <c r="C172" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -2508,6 +3026,9 @@
           <t>03-439</t>
         </is>
       </c>
+      <c r="C173" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -2520,6 +3041,9 @@
           <t>03-740</t>
         </is>
       </c>
+      <c r="C174" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -2532,6 +3056,9 @@
           <t>21-259</t>
         </is>
       </c>
+      <c r="C175" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -2544,6 +3071,9 @@
           <t>03-534</t>
         </is>
       </c>
+      <c r="C176" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -2556,6 +3086,9 @@
           <t>03-871</t>
         </is>
       </c>
+      <c r="C177" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -2568,6 +3101,9 @@
           <t>03-362</t>
         </is>
       </c>
+      <c r="C178" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -2580,6 +3116,9 @@
           <t>03-390</t>
         </is>
       </c>
+      <c r="C179" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -2592,6 +3131,9 @@
           <t>03-362</t>
         </is>
       </c>
+      <c r="C180" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -2604,6 +3146,9 @@
           <t>03-390</t>
         </is>
       </c>
+      <c r="C181" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -2616,6 +3161,9 @@
           <t>03-711</t>
         </is>
       </c>
+      <c r="C182" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -2628,6 +3176,9 @@
           <t>15-210</t>
         </is>
       </c>
+      <c r="C183" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -2640,6 +3191,9 @@
           <t>36-247</t>
         </is>
       </c>
+      <c r="C184" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -2652,6 +3206,9 @@
           <t>21-260</t>
         </is>
       </c>
+      <c r="C185" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -2664,6 +3221,9 @@
           <t>21-241</t>
         </is>
       </c>
+      <c r="C186" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -2676,6 +3236,9 @@
           <t>03-512</t>
         </is>
       </c>
+      <c r="C187" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -2688,6 +3251,9 @@
           <t>15-451</t>
         </is>
       </c>
+      <c r="C188" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -2700,6 +3266,9 @@
           <t>09-560</t>
         </is>
       </c>
+      <c r="C189" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -2712,6 +3281,9 @@
           <t>03-220</t>
         </is>
       </c>
+      <c r="C190" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -2724,6 +3296,9 @@
           <t>03-326</t>
         </is>
       </c>
+      <c r="C191" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -2736,6 +3311,9 @@
           <t>03-327</t>
         </is>
       </c>
+      <c r="C192" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -2748,6 +3326,9 @@
           <t>03-442</t>
         </is>
       </c>
+      <c r="C193" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -2760,6 +3341,9 @@
           <t>03-730</t>
         </is>
       </c>
+      <c r="C194" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -2772,6 +3356,9 @@
           <t>03-391</t>
         </is>
       </c>
+      <c r="C195" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -2784,6 +3371,9 @@
           <t>03-350</t>
         </is>
       </c>
+      <c r="C196" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -2796,6 +3386,9 @@
           <t>03-442</t>
         </is>
       </c>
+      <c r="C197" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -2808,6 +3401,9 @@
           <t>03-751</t>
         </is>
       </c>
+      <c r="C198" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -2820,6 +3416,9 @@
           <t>03-326</t>
         </is>
       </c>
+      <c r="C199" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -2832,6 +3431,9 @@
           <t>03-741</t>
         </is>
       </c>
+      <c r="C200" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -2844,6 +3446,9 @@
           <t>03-442</t>
         </is>
       </c>
+      <c r="C201" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -2856,6 +3461,9 @@
           <t>09-518</t>
         </is>
       </c>
+      <c r="C202" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -2868,6 +3476,9 @@
           <t>03-726</t>
         </is>
       </c>
+      <c r="C203" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -2880,6 +3491,9 @@
           <t>03-727</t>
         </is>
       </c>
+      <c r="C204" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -2892,6 +3506,9 @@
           <t>03-390</t>
         </is>
       </c>
+      <c r="C205" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -2904,6 +3521,9 @@
           <t>03-391</t>
         </is>
       </c>
+      <c r="C206" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -2916,6 +3536,9 @@
           <t>03-730</t>
         </is>
       </c>
+      <c r="C207" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -2928,6 +3551,9 @@
           <t>03-362</t>
         </is>
       </c>
+      <c r="C208" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -2940,6 +3566,9 @@
           <t>03-762</t>
         </is>
       </c>
+      <c r="C209" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -2952,6 +3581,9 @@
           <t>03-363</t>
         </is>
       </c>
+      <c r="C210" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -2964,6 +3596,9 @@
           <t>03-763</t>
         </is>
       </c>
+      <c r="C211" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -2976,6 +3611,9 @@
           <t>03-133</t>
         </is>
       </c>
+      <c r="C212" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -2988,6 +3626,9 @@
           <t>03-350</t>
         </is>
       </c>
+      <c r="C213" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -3000,6 +3641,9 @@
           <t>03-364</t>
         </is>
       </c>
+      <c r="C214" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -3012,6 +3656,9 @@
           <t>03-365</t>
         </is>
       </c>
+      <c r="C215" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -3024,6 +3671,9 @@
           <t>03-366</t>
         </is>
       </c>
+      <c r="C216" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -3036,6 +3686,9 @@
           <t>03-534</t>
         </is>
       </c>
+      <c r="C217" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -3048,6 +3701,9 @@
           <t>42-202</t>
         </is>
       </c>
+      <c r="C218" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -3059,6 +3715,9 @@
         <is>
           <t>85-219</t>
         </is>
+      </c>
+      <c r="C219" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>